<commit_message>
updated excel solar pv
</commit_message>
<xml_diff>
--- a/Modeling of solar PV/MA_2.xlsx
+++ b/Modeling of solar PV/MA_2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ZWL/GoogleDrive/2018spring/sys_mod/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\lib-public\PublicRedirected$\zl6444\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A4FDA20D-80A8-994C-9AC3-CECD123B1210}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Hours</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Variable cost of using batter($/kWh)</t>
   </si>
   <si>
-    <t>Battery Net output (kW)</t>
-  </si>
-  <si>
     <t>Installed Solar Capacity (kW)</t>
   </si>
   <si>
@@ -75,12 +72,21 @@
   </si>
   <si>
     <t>Total Output</t>
+  </si>
+  <si>
+    <t>Bus battery Net output</t>
+  </si>
+  <si>
+    <t>Station battery Net output (kW)</t>
+  </si>
+  <si>
+    <t>Charge port limit(kW)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -116,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,24 +439,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFDCD07-9E01-C14C-A188-7A3CBB99F3C2}">
-  <dimension ref="A1:Y22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -526,12 +534,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -608,69 +611,231 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>228</v>
+      </c>
+      <c r="C8">
+        <v>228</v>
+      </c>
+      <c r="D8">
+        <v>228</v>
+      </c>
+      <c r="E8">
+        <v>228</v>
+      </c>
+      <c r="F8">
+        <v>228</v>
+      </c>
+      <c r="G8">
+        <v>228</v>
+      </c>
+      <c r="H8">
+        <v>228</v>
+      </c>
+      <c r="I8">
+        <v>228</v>
+      </c>
+      <c r="J8">
+        <v>228</v>
+      </c>
+      <c r="K8">
+        <v>228</v>
+      </c>
+      <c r="L8">
+        <v>228</v>
+      </c>
+      <c r="M8">
+        <v>228</v>
+      </c>
+      <c r="N8">
+        <v>228</v>
+      </c>
+      <c r="O8">
+        <v>228</v>
+      </c>
+      <c r="P8">
+        <v>228</v>
+      </c>
+      <c r="Q8">
+        <v>228</v>
+      </c>
+      <c r="R8">
+        <v>228</v>
+      </c>
+      <c r="S8">
+        <v>228</v>
+      </c>
+      <c r="T8">
+        <v>228</v>
+      </c>
+      <c r="U8">
+        <v>228</v>
+      </c>
+      <c r="V8">
+        <v>228</v>
+      </c>
+      <c r="W8">
+        <v>228</v>
+      </c>
+      <c r="X8">
+        <v>228</v>
+      </c>
+      <c r="Y8">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>192</v>
+      </c>
+      <c r="J20">
+        <v>192</v>
+      </c>
+      <c r="K20">
+        <v>192</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>192</v>
+      </c>
+      <c r="Q20">
+        <v>192</v>
+      </c>
+      <c r="R20">
+        <v>192</v>
+      </c>
+      <c r="S20">
+        <v>192</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>